<commit_message>
Bank data collected.Card data ongoing
</commit_message>
<xml_diff>
--- a/data/Bank.xlsx
+++ b/data/Bank.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\NSU\CSE327\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\nsu.fall.2018.cse327.1.t2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9031C650-9F25-4B5C-91E0-341E7E36C8EA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C2B2766A-81EA-4756-845A-7C3710B736C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,55 +25,236 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>List of recommended banks</t>
-  </si>
-  <si>
-    <t>Dutch-Bangla Bank</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="74">
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Sonali Bank Limited</t>
+  </si>
+  <si>
+    <t>Janata Bank Limited</t>
+  </si>
+  <si>
+    <t>Agrani Bank Limited</t>
+  </si>
+  <si>
+    <t>Rupali Bank Limited</t>
+  </si>
+  <si>
+    <t>BASIC Bank Limited</t>
+  </si>
+  <si>
+    <t>Bangladesh Development Bank Limited</t>
+  </si>
+  <si>
+    <t>Bangladesh Krishi Bank</t>
+  </si>
+  <si>
+    <t>Rajshahi Krishi Unnayan Bank</t>
+  </si>
+  <si>
+    <t>Probashi Kallyan Bank</t>
+  </si>
+  <si>
+    <t>AB Bank Limited</t>
+  </si>
+  <si>
+    <t>Bangladesh Commerce Bank Limited</t>
+  </si>
+  <si>
+    <t>Bank Asia Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brac Bank Limited </t>
+  </si>
+  <si>
+    <t>City Bank Limited</t>
+  </si>
+  <si>
+    <t>Dhaka Bank Limited</t>
+  </si>
+  <si>
+    <t>Dutch Bangla Bank Limited</t>
   </si>
   <si>
     <t>Eastern Bank Limited</t>
   </si>
   <si>
-    <t>The City Bank Ltd.</t>
-  </si>
-  <si>
-    <t>Bank Asia Limited</t>
-  </si>
-  <si>
-    <t>BRAC Bank Limited</t>
-  </si>
-  <si>
-    <t>Dhaka Bank Ltd.</t>
-  </si>
-  <si>
-    <t>IFIC Bank Bangladesh Ltd.</t>
-  </si>
-  <si>
-    <t>AB Bank Limited</t>
+    <t>IFIC Bank Limited</t>
+  </si>
+  <si>
+    <t>Jamuna Bank Limited</t>
+  </si>
+  <si>
+    <t>Meghna Bank Limited</t>
+  </si>
+  <si>
+    <t>Mercantile Bank Limited</t>
+  </si>
+  <si>
+    <t>Midland Bank Limited</t>
+  </si>
+  <si>
+    <t>Modhumoti Bank Limited</t>
   </si>
   <si>
     <t>Mutual Trust Bank Limited</t>
   </si>
   <si>
-    <t xml:space="preserve">Standered Chartered Bank </t>
+    <t>National Bank Limited</t>
+  </si>
+  <si>
+    <t>National Credit and Commerce Bank Limited</t>
+  </si>
+  <si>
+    <t>NRB Bank Limited</t>
+  </si>
+  <si>
+    <t>NRB Commercial Bank Limited</t>
+  </si>
+  <si>
+    <t>NRB Global Bank Limited</t>
+  </si>
+  <si>
+    <t>One Bank Limited</t>
+  </si>
+  <si>
+    <t>Premier Bank Limited</t>
+  </si>
+  <si>
+    <t>Prime Bank Limited</t>
+  </si>
+  <si>
+    <t>Pubali Bank Limited</t>
+  </si>
+  <si>
+    <t>Shimanto Bank Limited</t>
+  </si>
+  <si>
+    <t>South Bangla Agriculture and Commerce Bank Limited</t>
+  </si>
+  <si>
+    <t>Southeast Bank Limited</t>
+  </si>
+  <si>
+    <t>Standard Bank Limited</t>
+  </si>
+  <si>
+    <t>Farmers Bank Limited</t>
+  </si>
+  <si>
+    <t>Trust Bank Limited</t>
+  </si>
+  <si>
+    <t>United Commercial Bank Limited</t>
+  </si>
+  <si>
+    <t>Uttara Bank Limited</t>
+  </si>
+  <si>
+    <t>Exim bank limited</t>
+  </si>
+  <si>
+    <t>First Security Islami Bank Limited</t>
+  </si>
+  <si>
+    <t>Shahjalal Islami Bank Limited</t>
+  </si>
+  <si>
+    <t>Social Islamic Bank Limited</t>
+  </si>
+  <si>
+    <t>Union Bank Limited</t>
+  </si>
+  <si>
+    <t>ICB Islami Bank Limited</t>
+  </si>
+  <si>
+    <t>Islami Bank Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>Al-Arafah Islaimi Bank Limited</t>
+  </si>
+  <si>
+    <t>Bank Al Falah Limited</t>
+  </si>
+  <si>
+    <t>Citibank  N.A</t>
+  </si>
+  <si>
+    <t>Commercial Bank of Ceylon PLC</t>
+  </si>
+  <si>
+    <t>Habib Bank Limited</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>National Bank of Pakistan</t>
+  </si>
+  <si>
+    <t>Standard Chartered Bank</t>
+  </si>
+  <si>
+    <t>State Bank of India</t>
+  </si>
+  <si>
+    <t>Woori Bank</t>
+  </si>
+  <si>
+    <t>Ansar VDP Unnayan Bank</t>
+  </si>
+  <si>
+    <t>Karmashangosthan Bank</t>
+  </si>
+  <si>
+    <t>Grameen Bank</t>
+  </si>
+  <si>
+    <t>Jubilee Bank</t>
+  </si>
+  <si>
+    <t>Palli Sanchay Bank</t>
+  </si>
+  <si>
+    <t>Bank Type</t>
+  </si>
+  <si>
+    <t>Bank Ownership</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>SOCB</t>
+  </si>
+  <si>
+    <t>SDB</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Islamic PCB</t>
+  </si>
+  <si>
+    <t>FCB</t>
+  </si>
+  <si>
+    <t>Non-Scheduled</t>
+  </si>
+  <si>
+    <t>Private</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,9 +282,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,7 +318,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -149,7 +330,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -166,9 +347,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -196,14 +377,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -231,6 +429,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,75 +597,736 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBE542F-C003-4121-A679-7A929BB90A14}">
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>